<commit_message>
upload Stage 1 and Stage 2: A1-A20
</commit_message>
<xml_diff>
--- a/GreenMit/evidence.xlsx
+++ b/GreenMit/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\CRYPTO FAMILY\NODES\Game NFT\7. GreenT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\CRYPTO FAMILY\NODES\Game NFT\0_7. GreenT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
   <si>
     <t>TxHash</t>
   </si>
@@ -57,45 +57,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -142,6 +109,207 @@
   </si>
   <si>
     <t>GreenT#5502</t>
+  </si>
+  <si>
+    <t>E83EAC12C3F3F8BEA174FEEEAB91B20F4E9EDEC3409FECF04AA83C0D4D32BAFA</t>
+  </si>
+  <si>
+    <t>greenNFT</t>
+  </si>
+  <si>
+    <t>EA4CDC5CB876E0D761C536345CABDD3ACA555F5BBB4A80E34420CBD330207FFF</t>
+  </si>
+  <si>
+    <t>green01</t>
+  </si>
+  <si>
+    <t>7D3AE45E15673BA54CEC9DF1265180F7B7A8B9F87FBF97EB5A14335D68576418</t>
+  </si>
+  <si>
+    <t>green02</t>
+  </si>
+  <si>
+    <t>4C6AB2CCE3F315172D1F7D6F873F3277F0EAEF19B0EC9A35313BA74D3119EE51</t>
+  </si>
+  <si>
+    <t>green03</t>
+  </si>
+  <si>
+    <t>39189D8841C99A379284493AEBEE7396B8B3C48B68AAEA8095141CCFCEE45BF2</t>
+  </si>
+  <si>
+    <t>wasm.juno12fcrjgmskednh690am3ydlwpfplrhsg3vfy6cq02vpmxjzd94ghqe3hj5u</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>2D2A7B5DA6C6C2B5104E71F21F507DB3E098F0CBB74EC9387C045F86C8E6C622</t>
+  </si>
+  <si>
+    <t>ibc/574E2619F13E7A72002C20A1A01F01CC03E2E024410B0BED51479BE0CE15EB97</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>6FF0F5D84C51704D234CA3B77AD7DCDE21D0A4FB1C2D57F3E29E5CB4572316D8</t>
+  </si>
+  <si>
+    <t>4F129B8666F152AC57F6E013AEA737FD0AB2D3C9B5453A3164A3CFEAEDFDC62E</t>
+  </si>
+  <si>
+    <t>ibc/8E0F85FE31A29AFA4D2B4497571AF569364AD5E0BE599DD84A292B92ACDE6A7A</t>
+  </si>
+  <si>
+    <t>green07</t>
+  </si>
+  <si>
+    <t>ibc/65B8B871BA2B7940D68960228ACE24BB84529E4C75ABCBA8C7CE8A3517228094</t>
+  </si>
+  <si>
+    <t>green08</t>
+  </si>
+  <si>
+    <t>ibc/05A884018E46FEFC68153F7FA20234FC66A384CBBDC1EC84B2372EC20AFBEA1D</t>
+  </si>
+  <si>
+    <t>green09</t>
+  </si>
+  <si>
+    <t>ibc/A2BE24191A84BA392FC23CB44410F23ABF4AC5BE525F4BF9DCD7BDFCEC66DE37</t>
+  </si>
+  <si>
+    <t>green010</t>
+  </si>
+  <si>
+    <t>ibc/988FA0A8ECF1B394B0312806DCB282E2F9EEC71D03B17477374DD52AAF8026C2</t>
+  </si>
+  <si>
+    <t>green011</t>
+  </si>
+  <si>
+    <t>ibc/0BCECE5EB500787A19F453175B47D01E71AAFC567E6E94A7D2C21416DE50529B</t>
+  </si>
+  <si>
+    <t>green012</t>
+  </si>
+  <si>
+    <t>8E50973C71E043603EAFA71C925CCD6FAFBD88129855C57BD8308852AE14E1A0</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>F43FE85AF436EE9260C138CC7CF4BA723DF6C4E8377F0EB2F8C002AB5AAB12A2</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>220A1CBBEB7201B5EB5C8A9D0E1FEA77F32A02AEEE08D6819826B6D82B461191</t>
+  </si>
+  <si>
+    <t>53E4B13F8CF23ED698DA3D540F17AEB43AE326F20D700905CDA540A6180F463A</t>
+  </si>
+  <si>
+    <t>764FA19CA764007E2FCE5C93F3A36E367036327CDB912B29CD6E66369B652A6D</t>
+  </si>
+  <si>
+    <t>96690FF9AF8ED35253F3DB3E434E6842AC9D019F75534F49DEC6F5226886A9AF</t>
+  </si>
+  <si>
+    <t>509CFF3F90B835724660B970D423A1B07FE6A9466E44D0C5E809627B6C06163A</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>E7EC1207A9C0B9EDC55DD4DACF6F572DA677B4B411BF728648F4D39410E99E56</t>
+  </si>
+  <si>
+    <t>03FE90254B82965696812FD1B150FBEEA2C68763A944720BE842149034977E0F</t>
+  </si>
+  <si>
+    <t>7D96D09B5DD726E07A2F51259679831E2330EF839828A024DECDEB4693E5DFD0</t>
+  </si>
+  <si>
+    <t>1BA22EEA6E9FF2004F459A8831F1C07D0211F10BD307D280104E1435AC49C189</t>
+  </si>
+  <si>
+    <t>C07E9AF9226019E8F0E0F009ACA657EF308EA08F118327E05AEB3AFCBA959EC0</t>
+  </si>
+  <si>
+    <t>2E238DA0AB467C1FC5BD45F6A133C5A37E1435ECE3F6C92C312AC7F714455A9C</t>
+  </si>
+  <si>
+    <t>9B6A954706A0EB6AF6D63FC92FB3D26D2A27137E88F13D0D1EF7D00C33C12BD8</t>
+  </si>
+  <si>
+    <t>E2D51A740B944CCB1D49B3EB7964CF16BCE2B2950301CED1A65E09306DEBD088</t>
+  </si>
+  <si>
+    <t>1F22A1A2A475532E7C887471FB9A54FCE85698AD826086DA16D8EC673FDDF160</t>
+  </si>
+  <si>
+    <t>F5173CBD8BEB7C358A403D5497C0F93C4044F5B3206358417DC9A1765FF28EDC</t>
+  </si>
+  <si>
+    <t>C00D2AC653B85BA825A2E7B6002B359C36353E0D4ABFFE745E95C32A71646F9F</t>
+  </si>
+  <si>
+    <t>BFE7A91FA967063456E3E671F2BF86E1B14C3F95DC0180791BF9721140626025</t>
+  </si>
+  <si>
+    <t>58DED6D0A6DA03ABB165000B7C31AE17F9A272203201BCD3CFC0011ED5AD6338</t>
+  </si>
+  <si>
+    <t>EAC2A5459A0664BF7B18467A00A8E5B92CC496EDFDDAE1F2926F979FE7618A57</t>
+  </si>
+  <si>
+    <t>747A8A387EDD5DBA39B71DF699619258799DB92FB2F4D546E559DA37DA0EC9C9</t>
+  </si>
+  <si>
+    <t>E59FD42E6825CF9DD5A80BEAF85BE9CD9CF1C6ECA986F9E8F148B30969FF0F99</t>
+  </si>
+  <si>
+    <t>D7ED8DE49B7CAAA13FCFEB4C5FDD83914C9050D25197E441E1B8D7C09CF1B4CD</t>
+  </si>
+  <si>
+    <t>2CF8721A8F7B793AB7A2BDF483E909FCB1018477EA5E64B74D4FA14D8711E193</t>
+  </si>
+  <si>
+    <t>2EC40A51349BDC717FB11D3BA15E8E913B228FDE132D25DF95779F75750622EA</t>
+  </si>
+  <si>
+    <t>F0753A304E4BA06BC8598A4113DE2FABF4A2C146092C4A4843C166B3972F2C96</t>
+  </si>
+  <si>
+    <t>2E27514DC4A73D66EB899F2C3127489EA65DDC8BC079C282CE46A151163E8A2D</t>
+  </si>
+  <si>
+    <t>C104546D46B3B4A55C336CEDE718276755683E0795FF4609F5FBA2E4D385BDBD</t>
+  </si>
+  <si>
+    <t>BDD781D1AE90A53EFD3A292C50D7D2E2A0BADF6BB2A9D6831C4A3284E3B12D32</t>
+  </si>
+  <si>
+    <t>66E9A1F15869F4D6181A71C744DD8D21747A0FA3382EA2AB8664F167C6028A97</t>
+  </si>
+  <si>
+    <t>20386D4C57FD677C0782190B85EFDC1EA519B432E0E270DDCB82BE508611CD68</t>
+  </si>
+  <si>
+    <t>8CFAC504BB100BD36961D947CCF115FE86B97D5BF46A4811AB436401B81BC3BA</t>
+  </si>
+  <si>
+    <t>FE17B64EBE94147CEC5C7B522C855270992E6A50298203FEA739D531255AF87A</t>
+  </si>
+  <si>
+    <t>E88F5CF6A6A4DE0C6F4D396DB58C7FBF21277F3A32BF21A8886F678D00E2F9DC</t>
+  </si>
+  <si>
+    <t>2A3D2065FEDBAD86795F81A651B5C3066DAF48AF954C287B599D0F3C06A47173</t>
   </si>
 </sst>
 </file>
@@ -539,7 +707,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,54 +724,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -619,7 +787,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -629,18 +799,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -655,7 +825,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -665,18 +837,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -691,7 +863,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -701,18 +875,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -727,7 +901,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -737,18 +913,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -761,9 +937,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -781,23 +959,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -809,9 +999,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -829,23 +1021,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -857,9 +1061,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -877,23 +1083,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -905,9 +1123,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -925,23 +1145,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -953,9 +1185,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -973,23 +1207,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1001,9 +1247,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1021,23 +1269,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1051,7 +1311,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1063,19 +1325,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1084,9 +1347,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1104,23 +1369,55 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1132,9 +1429,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1152,23 +1451,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1316,9 +1643,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1331,21 +1660,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1360,7 +1711,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1374,10 +1727,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1385,16 +1738,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1409,7 +1762,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1423,10 +1778,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1434,16 +1789,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1458,7 +1813,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1472,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1483,16 +1840,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1507,7 +1864,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1522,10 +1881,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1533,16 +1892,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1557,7 +1916,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1567,22 +1928,23 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1593,7 +1955,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1603,18 +1967,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>